<commit_message>
adição de "Dirigindo meu carro no arquivo"
</commit_message>
<xml_diff>
--- a/PastaModelosBD/Book1.xlsx
+++ b/PastaModelosBD/Book1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\logonrmlocal\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1CED1801-21FD-4FDB-B9B4-57B7728B9ADF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C0FEDF-7AFD-44C2-AA36-9EAFAE364E06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11385" xr2:uid="{3E7351B9-50E6-4806-93ED-D7BB3E5DE74F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>REQUISITO</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>cada cliente so visualiza seus pontos</t>
+  </si>
+  <si>
+    <t>DIRIGINDO MEU CARRO</t>
   </si>
 </sst>
 </file>
@@ -527,7 +530,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,7 +654,9 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>

</xml_diff>